<commit_message>
Integration-Matlab-Python for color transfer
Almost done without terminal…
so far it is needed to run
python DOTSolver.py "algorithm-" "out_folder/"
</commit_message>
<xml_diff>
--- a/Python Algorithms/Test/DR-Critical.xlsx
+++ b/Python Algorithms/Test/DR-Critical.xlsx
@@ -420,22 +420,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0.03240427819371842</v>
+        <v>0.00275442249619973</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0.9914352118230582</v>
+        <v>0.9514223331899243</v>
       </c>
       <c r="F2">
-        <v>0.02038097381591797</v>
+        <v>0.003188848495483398</v>
       </c>
       <c r="G2">
-        <v>0.7865187977445212</v>
+        <v>0.9960679680569756</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -443,22 +443,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>564</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>0.01789732206946931</v>
+        <v>0.05158144172721063</v>
       </c>
       <c r="D3">
         <v>0.1</v>
       </c>
       <c r="E3">
-        <v>0.09989666035481098</v>
+        <v>0.09029711554240791</v>
       </c>
       <c r="F3">
-        <v>0.1177330017089844</v>
+        <v>0.01740074157714844</v>
       </c>
       <c r="G3">
-        <v>0.4807156815691971</v>
+        <v>0.9758368432954937</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -466,22 +466,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1417</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>0.01643419992442831</v>
+        <v>0.0566794055335246</v>
       </c>
       <c r="D4">
         <v>0.01</v>
       </c>
       <c r="E4">
-        <v>0.009979121028242775</v>
+        <v>0.0003881827136121285</v>
       </c>
       <c r="F4">
-        <v>0.2769749164581299</v>
+        <v>0.02093791961669922</v>
       </c>
       <c r="G4">
-        <v>0.3828314770520149</v>
+        <v>0.9669067670575243</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -489,22 +489,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2039</v>
+        <v>4371</v>
       </c>
       <c r="C5">
-        <v>0.01628751825093378</v>
+        <v>0.05675808555049239</v>
       </c>
       <c r="D5">
         <v>0.001</v>
       </c>
       <c r="E5">
-        <v>0.0009646616479142413</v>
+        <v>0.0009994372517873483</v>
       </c>
       <c r="F5">
-        <v>0.3918840885162354</v>
+        <v>2.680588722229004</v>
       </c>
       <c r="G5">
-        <v>0.3641439368645042</v>
+        <v>0.6006062222089232</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -512,22 +512,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2062</v>
+        <v>21724</v>
       </c>
       <c r="C6">
-        <v>0.0162731950836625</v>
+        <v>0.05670708231967949</v>
       </c>
       <c r="D6">
         <v>0.0001</v>
       </c>
       <c r="E6">
-        <v>8.44180122333965E-05</v>
+        <v>9.993183601156125E-05</v>
       </c>
       <c r="F6">
-        <v>0.3963649272918701</v>
+        <v>13.74774575233459</v>
       </c>
       <c r="G6">
-        <v>0.3634732519939692</v>
+        <v>0.3598264157717663</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -535,22 +535,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2065</v>
+        <v>82212</v>
       </c>
       <c r="C7">
-        <v>0.01627173922753292</v>
+        <v>0.05670198197752034</v>
       </c>
       <c r="D7">
         <v>1E-05</v>
       </c>
       <c r="E7">
-        <v>5.05298732037594E-06</v>
+        <v>9.98095797220148E-06</v>
       </c>
       <c r="F7">
-        <v>0.3971760272979736</v>
+        <v>53.45275068283081</v>
       </c>
       <c r="G7">
-        <v>0.3633874641644878</v>
+        <v>0.1776273892192539</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -558,22 +558,22 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>3146</v>
+        <v>190229</v>
       </c>
       <c r="C8">
-        <v>0.01627183188524661</v>
+        <v>0.05670147271032179</v>
       </c>
       <c r="D8">
         <v>1E-06</v>
       </c>
       <c r="E8">
-        <v>6.413791020025549E-07</v>
+        <v>9.993974735381498E-07</v>
       </c>
       <c r="F8">
-        <v>0.5984029769897461</v>
+        <v>118.4360136985779</v>
       </c>
       <c r="G8">
-        <v>0.3589295985423676</v>
+        <v>0.09369313456201694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>